<commit_message>
add for ex week 2
</commit_message>
<xml_diff>
--- a/lecture/week2课堂练习.xlsx
+++ b/lecture/week2课堂练习.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4515" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4515"/>
   </bookViews>
   <sheets>
     <sheet name="PCA" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>C1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,6 +108,10 @@
   </si>
   <si>
     <t>Sw = S1+S2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCA是非监督的，实际无C1、C2标签，所以把C1、C2混合起来计算</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -465,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -476,7 +480,7 @@
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -484,7 +488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -495,7 +499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>2</v>
       </c>
@@ -503,7 +507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>3</v>
       </c>
@@ -511,7 +515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>4</v>
       </c>
@@ -519,7 +523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>5</v>
       </c>
@@ -527,7 +531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -538,7 +542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>2</v>
       </c>
@@ -546,7 +550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>3</v>
       </c>
@@ -554,7 +558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>3</v>
       </c>
@@ -562,7 +566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>5</v>
       </c>
@@ -570,7 +574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>6</v>
       </c>
@@ -578,7 +582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -588,8 +592,11 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>6</v>
       </c>
@@ -597,7 +604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16">
         <f>_xlfn.COVARIANCE.S(B2:B12,B2:B12)</f>
         <v>2.7636363636363628</v>
@@ -638,7 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>

</xml_diff>